<commit_message>
chapter III is completed.
</commit_message>
<xml_diff>
--- a/数据.xlsx
+++ b/数据.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20341"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20344"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABEACE02EC09BB9C73525BDE589D" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{AA0346FA-2AEA-4604-A866-81828F41728A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F3DF71-BD62-495F-B34D-9C4A8FAB13CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="图片数据" sheetId="1" r:id="rId1"/>
+    <sheet name="数据分布" sheetId="2" r:id="rId1"/>
+    <sheet name="图片切割数据" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>handled</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,12 +50,36 @@
     <t>test-rust</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>train</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>evluate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>叶枯病</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>白粉病</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>锈病</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +91,13 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -110,6 +142,1225 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN"/>
+              <a:t>数据分布</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>数据分布!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>train</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>数据分布!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>叶枯病</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>白粉病</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>锈病</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>数据分布!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9CF3-433E-9545-724035823591}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>数据分布!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>数据分布!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>叶枯病</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>白粉病</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>锈病</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>数据分布!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>174</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9CF3-433E-9545-724035823591}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>数据分布!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evluate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>数据分布!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>叶枯病</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>白粉病</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>锈病</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>数据分布!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>174</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9CF3-433E-9545-724035823591}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="37196304"/>
+        <c:axId val="161578384"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="37196304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="161578384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="161578384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37196304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>71628</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE8403E4-DF97-41DD-BAB0-02D5D3FF06B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -374,10 +1625,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10E7FF1-6A29-4876-8725-FB4CF0BF921F}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>278</v>
+      </c>
+      <c r="C2" s="1">
+        <v>94</v>
+      </c>
+      <c r="D2" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>337</v>
+      </c>
+      <c r="C3" s="1">
+        <v>111</v>
+      </c>
+      <c r="D3" s="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>525</v>
+      </c>
+      <c r="C4" s="1">
+        <v>174</v>
+      </c>
+      <c r="D4" s="1">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>